<commit_message>
Again, another update with the new analysis system.
</commit_message>
<xml_diff>
--- a/Stress_and_Yoga/SR_data_50_73_80.xlsx
+++ b/Stress_and_Yoga/SR_data_50_73_80.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9a6b3eff62ff7c65/Desktop/Stress/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter\bacn_lab\Stress_and_Yoga\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A803268E-A361-45BA-AEF4-2822918642C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD011E8-37DF-4128-AB51-49F49BD887EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" xr2:uid="{0DD74A98-5662-4D11-9AB7-6C181D6CEAED}"/>
+    <workbookView xWindow="368" yWindow="368" windowWidth="14399" windowHeight="8272" xr2:uid="{0DD74A98-5662-4D11-9AB7-6C181D6CEAED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
   <si>
     <t>SR</t>
   </si>
@@ -430,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{053932AE-041C-4E43-A1EB-33FAE9461BF9}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -441,26 +441,26 @@
     <col min="2" max="2" width="9.06640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -577,6 +577,121 @@
       </c>
       <c r="G6" s="2">
         <v>6.0958899999999997E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>73</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1">
+        <v>67.992369999999994</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.773567</v>
+      </c>
+      <c r="E7" s="2">
+        <v>6.2268500000000002E-5</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1.61633E-4</v>
+      </c>
+      <c r="G7" s="1">
+        <v>2.0894500000000001E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>73</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1">
+        <v>70.476900000000001</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.422593</v>
+      </c>
+      <c r="E8" s="2">
+        <v>2.7780600000000002E-7</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1.0250999999999999E-6</v>
+      </c>
+      <c r="G8" s="2">
+        <v>2.42575E-6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>73</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="1">
+        <v>68.067750000000004</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1.0098199999999999</v>
+      </c>
+      <c r="E9" s="2">
+        <v>7.7207300000000002E-5</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1.7866400000000001E-4</v>
+      </c>
+      <c r="G9" s="1">
+        <v>1.7692599999999999E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>73</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="1">
+        <v>70.51576</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1.2548699999999999</v>
+      </c>
+      <c r="E10" s="2">
+        <v>4.3641199999999998E-5</v>
+      </c>
+      <c r="F10" s="1">
+        <v>2.01883E-4</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1.6087999999999999E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>73</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="1">
+        <v>69.109520000000003</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1.8723099999999999</v>
+      </c>
+      <c r="E11" s="2">
+        <v>3.6699599999999997E-5</v>
+      </c>
+      <c r="F11" s="1">
+        <v>3.4311299999999998E-4</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1.8325000000000001E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
all analysis variables taken from biopac software
</commit_message>
<xml_diff>
--- a/Stress_and_Yoga/SR_data_50_73_80.xlsx
+++ b/Stress_and_Yoga/SR_data_50_73_80.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter\bacn_lab\Stress_and_Yoga\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD011E8-37DF-4128-AB51-49F49BD887EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D93B3C-3746-4A5B-805E-0251ED722F4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="368" yWindow="368" windowWidth="14399" windowHeight="8272" xr2:uid="{0DD74A98-5662-4D11-9AB7-6C181D6CEAED}"/>
+    <workbookView xWindow="1440" yWindow="1440" windowWidth="14400" windowHeight="8272" xr2:uid="{0DD74A98-5662-4D11-9AB7-6C181D6CEAED}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ALL_Trials" sheetId="1" r:id="rId1"/>
+    <sheet name="SR_50" sheetId="2" r:id="rId2"/>
+    <sheet name="SR_73" sheetId="3" r:id="rId3"/>
+    <sheet name="SR_80" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="12">
   <si>
     <t>SR</t>
   </si>
@@ -430,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{053932AE-041C-4E43-A1EB-33FAE9461BF9}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -694,8 +697,528 @@
         <v>1.8325000000000001E-4</v>
       </c>
     </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>80</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="1">
+        <v>92.535939999999997</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1.6275200000000001</v>
+      </c>
+      <c r="E12" s="2">
+        <v>9.8082599999999995E-6</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1.1613900000000001E-5</v>
+      </c>
+      <c r="G12" s="2">
+        <v>7.13594E-6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>80</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="1">
+        <v>93.091489999999993</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.40773500000000001</v>
+      </c>
+      <c r="E13" s="2">
+        <v>2.21612E-8</v>
+      </c>
+      <c r="F13" s="2">
+        <v>8.22794E-8</v>
+      </c>
+      <c r="G13" s="2">
+        <v>2.0179599999999999E-7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A14">
+        <v>80</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="1">
+        <v>91.609089999999995</v>
+      </c>
+      <c r="D14" s="1">
+        <v>2.6861700000000002</v>
+      </c>
+      <c r="E14" s="2">
+        <v>7.6282299999999996E-6</v>
+      </c>
+      <c r="F14" s="2">
+        <v>2.5930200000000001E-5</v>
+      </c>
+      <c r="G14" s="2">
+        <v>9.65321E-6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A15">
+        <v>80</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="1">
+        <v>92.212890000000002</v>
+      </c>
+      <c r="D15" s="1">
+        <v>2.7179799999999998</v>
+      </c>
+      <c r="E15" s="2">
+        <v>5.2319599999999998E-6</v>
+      </c>
+      <c r="F15" s="2">
+        <v>2.1852799999999999E-5</v>
+      </c>
+      <c r="G15" s="2">
+        <v>8.0400700000000008E-6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>80</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="1">
+        <v>91.163510000000002</v>
+      </c>
+      <c r="D16" s="1">
+        <v>2.8380200000000002</v>
+      </c>
+      <c r="E16" s="2">
+        <v>4.1753399999999999E-6</v>
+      </c>
+      <c r="F16" s="2">
+        <v>2.7167099999999999E-5</v>
+      </c>
+      <c r="G16" s="2">
+        <v>9.5725500000000004E-6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AD4008F-B9B6-486B-B200-7D2ED885D57F}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>74.501090000000005</v>
+      </c>
+      <c r="C2" s="1">
+        <v>77.308779999999999</v>
+      </c>
+      <c r="D2" s="1">
+        <v>72.039670000000001</v>
+      </c>
+      <c r="E2" s="1">
+        <v>76.686089999999993</v>
+      </c>
+      <c r="F2" s="1">
+        <v>74.745310000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1.5268699999999999</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.43846800000000002</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.79209399999999996</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1.8745499999999999</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2.0908699999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1.1759799999999999E-4</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3.51446E-11</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2.7319300000000003E-4</v>
+      </c>
+      <c r="E4" s="1">
+        <v>6.27471E-4</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2.6356799999999999E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1.3293800000000001E-4</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1.2892300000000001E-10</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1.54337E-4</v>
+      </c>
+      <c r="E5" s="1">
+        <v>4.7692200000000001E-4</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1.2745700000000001E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2">
+        <v>8.7065199999999994E-5</v>
+      </c>
+      <c r="C6" s="2">
+        <v>2.9403199999999998E-10</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1.94847E-4</v>
+      </c>
+      <c r="E6" s="1">
+        <v>2.5441999999999999E-4</v>
+      </c>
+      <c r="F6" s="2">
+        <v>6.0958899999999997E-5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1E49F3B-CEEE-460B-AD41-948BD34422A3}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>67.992369999999994</v>
+      </c>
+      <c r="C2" s="1">
+        <v>70.476900000000001</v>
+      </c>
+      <c r="D2" s="1">
+        <v>68.067750000000004</v>
+      </c>
+      <c r="E2" s="1">
+        <v>70.51576</v>
+      </c>
+      <c r="F2" s="1">
+        <v>69.109520000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.773567</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.422593</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1.0098199999999999</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1.2548699999999999</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1.8723099999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>6.2268500000000002E-5</v>
+      </c>
+      <c r="C4" s="2">
+        <v>2.7780600000000002E-7</v>
+      </c>
+      <c r="D4" s="2">
+        <v>7.7207300000000002E-5</v>
+      </c>
+      <c r="E4" s="2">
+        <v>4.3641199999999998E-5</v>
+      </c>
+      <c r="F4" s="2">
+        <v>3.6699599999999997E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1.61633E-4</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1.0250999999999999E-6</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1.7866400000000001E-4</v>
+      </c>
+      <c r="E5" s="1">
+        <v>2.01883E-4</v>
+      </c>
+      <c r="F5" s="1">
+        <v>3.4311299999999998E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2.0894500000000001E-4</v>
+      </c>
+      <c r="C6" s="2">
+        <v>2.42575E-6</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1.7692599999999999E-4</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1.6087999999999999E-4</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1.8325000000000001E-4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8691301-2C1A-4F69-BA42-656D289949A1}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>92.535939999999997</v>
+      </c>
+      <c r="C2" s="1">
+        <v>93.091489999999993</v>
+      </c>
+      <c r="D2" s="1">
+        <v>91.609089999999995</v>
+      </c>
+      <c r="E2" s="1">
+        <v>92.212890000000002</v>
+      </c>
+      <c r="F2" s="1">
+        <v>91.163510000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1.6275200000000001</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.40773500000000001</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2.6861700000000002</v>
+      </c>
+      <c r="E3" s="1">
+        <v>2.7179799999999998</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2.8380200000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>9.8082599999999995E-6</v>
+      </c>
+      <c r="C4" s="2">
+        <v>2.21612E-8</v>
+      </c>
+      <c r="D4" s="2">
+        <v>7.6282299999999996E-6</v>
+      </c>
+      <c r="E4" s="2">
+        <v>5.2319599999999998E-6</v>
+      </c>
+      <c r="F4" s="2">
+        <v>4.1753399999999999E-6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1.1613900000000001E-5</v>
+      </c>
+      <c r="C5" s="2">
+        <v>8.22794E-8</v>
+      </c>
+      <c r="D5" s="2">
+        <v>2.5930200000000001E-5</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2.1852799999999999E-5</v>
+      </c>
+      <c r="F5" s="2">
+        <v>2.7167099999999999E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2">
+        <v>7.13594E-6</v>
+      </c>
+      <c r="C6" s="2">
+        <v>2.0179599999999999E-7</v>
+      </c>
+      <c r="D6" s="2">
+        <v>9.65321E-6</v>
+      </c>
+      <c r="E6" s="2">
+        <v>8.0400700000000008E-6</v>
+      </c>
+      <c r="F6" s="2">
+        <v>9.5725500000000004E-6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>